<commit_message>
results of NUC sensitivities updated
</commit_message>
<xml_diff>
--- a/ESM_Italy_7/case_studies/Italy24/scenarios/b.1_NUC_7/inputs/TechnologyData.xlsx
+++ b/ESM_Italy_7/case_studies/Italy24/scenarios/b.1_NUC_7/inputs/TechnologyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\ESM-Italy\ESM_Italy_7\case_studies\Italy24\scenarios\b.1_NUC_7\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002DDF7B-B315-40A2-9BE7-598DC2AA65D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7BF89F-43BF-4EC2-B1F9-C7316A9C971A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="r.A.T1" sheetId="1" r:id="rId1"/>
@@ -3037,11 +3037,11 @@
   <dimension ref="A1:AG55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="Z20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="O20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I9" sqref="I9"/>
       <selection pane="topRight" activeCell="I9" sqref="I9"/>
       <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
-      <selection pane="bottomRight" activeCell="Q44" sqref="Q44"/>
+      <selection pane="bottomRight" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>